<commit_message>
Get daily reddit data: Tue Jun  4 08:08:47 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_09.xlsx
+++ b/data/2024_06_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C477"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5552,6 +5552,2999 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1d7rf4h</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>questions regarding nail paints</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7rf4h/questions_regarding_nail_paints/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1d7py42</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Happy Pride! 🌈</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bo3qsucnuh4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1d7q613</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Juicy Orange Nails for Summer</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mwm05mn4xh4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1d7pyv6</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>How to use a nail strengthener?</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7pyv6/how_to_use_a_nail_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1d7pmr2</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>What can I do with my short nails??</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7pmr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1d7oori</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Advice on Broken Nail Drill</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7oori/advice_on_broken_nail_drill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1d7oksr</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>Favorite white/black polishes?</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7oksr/favorite_whiteblack_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1d7ojd4</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Went a bit different from my usual and opted for short and pink. </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2xkj5ug2fh4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1d7o7sm</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>nails for my birthday today !!</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7o7sm</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1d7o2z9</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails for a Melanie Martinez concert </t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7o2z9</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1d7nz06</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Can I sit in the comfy salon chairs and get a pedicure at the same time as getting a fill?</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7nz06/can_i_sit_in_the_comfy_salon_chairs_and_get_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1d7nigd</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pretty cute </t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bjnfvlhq4h4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1d7ngel</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>So proud of these ones! 🤌🏻</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7ngel</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1d7nat6</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>My shellac is chipping off at 1.5 weeks</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7nat6/my_shellac_is_chipping_off_at_15_weeks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1d7n6en</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>first ever set 😍💕</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7n6en</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1d7mmb4</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glamnetics for the win! </t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ddctqj8wg4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1d7mizd</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>🌈 nails for pride month!</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7mizd</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1d7m72i</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Some of my favorite nails I’ve done!As you can tell I love matching nails to other things. All done with gel, self taught</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7m72i</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1d7ljz7</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>all the nails I made &amp; wore in Japan!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7ljz7</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1d7ljg9</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My pride nails </t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zijwcacemg4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1d7l6gg</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Happy pride month</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cz81pbn0jg4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1d7ktjo</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanting to become a nail tech. </t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7ktjo/wanting_to_become_a_nail_tech/</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1d7ks3l</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving my new nail polish 😍 </t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p46wm7idfg4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1d7kqzm</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Sequin nails</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7kqzm</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1d7kotf</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Marble Nails</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d16vkyvleg4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1d7knxc</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Dainty Glue On Set</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7knxc</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1d7ke5b</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Wedding guest season!</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mibuwvbzbg4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1d7jlg8</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>A coworker said my pink nails clashed with my uniform, so this time I matched</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uzk18j7v4g4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1d7jgqf</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Are these fake nails hideous?</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7jgqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1d7jbyg</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Tangerines! 🍊</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7jbyg</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1d7j60k</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Press ons for wide thumbs?</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8zfuq2z81g4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1d7ix7h</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>idk what to do</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzz48h63zf4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1d7i51q</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Nail day for one of my babies 🥰</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n3ce2diosf4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1d7i107</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Gel Extensions + Mooncat Merkitten Polish</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7i107</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1d7hykr</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Simple but beautiful</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgupq858rf4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1d7hg7e</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Cat eye nails</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hbyy9ln3nf4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1d7hcad</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Glitter Flakes</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9eo7rp8mf4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1d7hbdz</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Should I cut my nails to size before my appointment?</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7hbdz/should_i_cut_my_nails_to_size_before_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1d7h94i</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>What do you think of these press ons?</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7h94i</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1d7h5og</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>I absolutely love this set</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7h5og</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1d7h2tb</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Do these nail shape and color harmonize with my skin?</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7h2tb</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1d7gy90</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>Very excited to show you guys this set I did on my friend today</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7gy90</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1d7gw18</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Best Manicure Method</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7gw18/best_manicure_method/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1d7gtz0</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Summery Acrylic Nails</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zsw4iu5aif4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1d7gp4q</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red Nails </t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7gp4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1d7go7h</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Perfect color (and cat toy🍦) for summer 😋</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7go7h</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1d7gf50</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Press-ons for small nail beds?</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7gf50/pressons_for_small_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1d7gdiw</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Same length nails by Nailcou on youtube</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyz4578sef4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1d7gb15</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Nail drill recommendations?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7gb15/nail_drill_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1d7g418</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Just finished my Pride nails! 🧡🤍🩷</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7g418</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1d7g2xc</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>favorite kind of green?</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmne87rkcf4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1d7ftkj</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Did my friends nails</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7ftkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1d7fpcq</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gel x lifting </t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7fpcq/gel_x_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1d7foom</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>SUMMERRRR</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hylsms0o9f4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1d7fhwg</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my mom today! </t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7fhwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1d7fdu2</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set, why don’t I love it? </t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7fdu2</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1d7fat4</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Italian summer vibes 🍊</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/djv7dj2u6f4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1d7f5sy</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Stitch set made by me ✨💕</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o1ulmptt5f4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1d7f5ss</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>New set 💛</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12viyhrt5f4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1d7eyz6</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>Worth it?</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gor370bf4f4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1d7ehea</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Teen nail artist here😁</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqeqvnox0f4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1d7dzl3</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Just some fun blue I wanted to share!</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7y3anrdjxe4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1d7dzaa</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Some of my favorite sets I've done the past year</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7dzaa</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1d7dvqi</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Glow in the dark (and color changing) set!</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7dvqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1d7dlb4</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Finally found a green I’ve been looking for!</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7dlb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1d7d8b5</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The picture does not do the glitter justice! </t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mput9mp9se4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1d7d61m</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>Good to have a palette cleanser every now and then.</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5g6sbgture4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1d7d5so</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>The perfect nails for minnie mouse don't exi...</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7d5so</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1d7d0l6</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my nails! </t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7d0l6</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1d7cdbu</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>What’s going on with my nails? Lunula going deeper down nail and weird shape</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7cdbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1d7c7lu</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Last summers lavender nails</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jutnnmy2le4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1d7c5z3</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Miss this shape</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nb0tpjckke4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1d7c3sy</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Silver chrome</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ijli5eake4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1d7by53</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Builder Gel in a Bottle!</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7by53</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1d7bu8c</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Help with Shape?</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p46gewbdie4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1d7bty2</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>My vacation nails 🤩</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/18nrvglbie4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1d7bfo1</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>would they do it? 💜💜</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v3jusj7ife4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1d7bcz1</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>After vs before</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7bcz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1d7b2u0</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>This go around, something sweet! 🍒 What do you guys think? Too childish?</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7b2u0</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1d7b1yk</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>🧚🏽‍♀️</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7b1yk</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1d7anye</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>nail sets from last year</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7anye</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1d7abpp</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Super spring vibes lol</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/od7181jj7e4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1d7aa1t</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Am I doing this right</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7aa1t/am_i_doing_this_right/</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1d7a7d1</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I was feeling zero creative and this is how it turned out 🤷🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9qfk63m6e4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1d7a4sm</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>My friend did her nails today</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol9r74p36e4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1d7a4an</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>I couldnt ask for better nails. Lasted all weekend AND Monday at work. Highly recommend OPI Xpress/on</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7a4an</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1d7a14c</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Koi pond 🪷✨ hand painted gel on myself</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7a14c</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1d79x4v</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>I haven’t cleaned up yet, but this was my first time using stickers and powder, and I’m obsessed</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83j80yzi4e4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1d79x45</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>My birthday set from this year</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d79x45</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1d79tk3</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>OPI Cajun Shrimp gel with a little gold leaf accent, I love them!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flq66xus3e4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1d79qen</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>It’s my first time getting semipermanent nails</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jcjcyaw53e4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1d79c29</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Pride nails! 🌈</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f7ho06k80e4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1d79259</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t xml:space="preserve">are the nails too long? feel like my hand could looks a bit disproportionate. any tips? </t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3jjaym8yd4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1d78y7b</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>I’ve just came from my nail tech appointment happy af!</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d78y7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1d78www</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>i got my nails done for graduation 🩷</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d78www</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1d78f19</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>mermaid scales - finished and cleaned up 🧜🏻✨🐠</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sau46ktktd4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1d78dyb</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Im not used to doing light colors, do they look odd with my skin tone? </t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d78dyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1d77gdr</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Cottage themed stamps and tulips 💕</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d77gdr</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1d77g6w</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Husband’s Choice</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d77g6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1d779hd</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>First set ever done by myself (painting with your non dominant hand is hard how do yall do it?)</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d779hd</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1d7rf1p</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Mylee products not creating peeling but Mack’s does? What’s a winning combo?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7rf1p</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1d7gozb</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with nail-bed growth </t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hkir8r6hf4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1d77joa</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>first time doing french tips ✨</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l4i7g6fbnd4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1d74wvy</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Do you need to have an account/membership for polish pickup?</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d74wvy/do_you_need_to_have_an_accountmembership_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1d7059q</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Hello guys can u decide what is my skin undertone? according to my veins</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1j2bpnppb4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1d7q1b3</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Happy Pride! 🌈</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e18rfh9ovh4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1d7ny93</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Iris You Were Here 😁💕</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7ny93</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1d7nfe8</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>🏎️💨</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7nfe8</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1d7msdt</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Blackheart Nail Polish</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bw4m6thuxg4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1d7kd1k</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Nail day for one of my babies 🥰</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojlguuepbg4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1d7k5xz</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>My first order from Lurid Lacquer ✨</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsds6g4z9g4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1d7jpyr</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Are dark shades of mooncat polish easy to take off</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d7jpyr/are_dark_shades_of_mooncat_polish_easy_to_take_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1d7ia7j</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>wow this polish has lasted me 6 days through work and using my hands roughly this week 😂 !!! it’s either the new prep i’m doing or it’s the polish ..either way shoutout to mooncat ! i’ve never had a mani last this long!!</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fnbl5z6utf4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1d7hms4</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>I'M IN LOVE</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x6upg85jof4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1d7h5mn</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Entirely obsessed</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7h5mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1d7glhm</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>MoYou London is phasing out their stamping plates and supplies in favor of gel nail strips! (😭😭)</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xa2knv7ggf4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1d7g1oe</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>My latest nails, French with autumn colors, do you like it? ❤️💗</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d6l16gbcf4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1d7fxqq</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Delphinus by Cirque Colors (horseshoe magnet velvet effect)</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ki76b59ebf4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1d7f1tb</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Oh Aspen 🌳</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7f1tb</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1d7e5dj</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Found this in the archives… who remembers Eyeko?</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sboz6cdnye4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1d7e4wq</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Glowy pseudo rainbow...</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7e4wq</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1d7diov</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>The rainbowiest non-holo rainbow I’ve found to date</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7diov</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1d7ccfa</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thermals </t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d7ccfa/thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1d7bzvm</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Okay everyone was right about the big horseshoe magnets—</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8cdsudyhje4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1d7blbl</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Alone isn't so bad, I like alone</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/atihngnlge4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1d7bgke</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Swamp Gloss - Always has been</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7bgke</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1d7bb24</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>I was so close to saying no to this polish, thank God.</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7bb24</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1d7aytj</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>🧚🏽‍♀️</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7aytj</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1d7adpb</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Looking for a sticky base coat alternative to ORLY Bonder</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d7adpb/looking_for_a_sticky_base_coat_alternative_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1d7ac3b</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Strawberry jelly nails</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqpi4b4m7e4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1d7a9w6</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Opinion on OPI Nail Polish</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d7a9w6/opinion_on_opi_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1d7a92t</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Am I doing this right</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d7a92t/am_i_doing_this_right/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1d79zuu</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>I wanted to post my nails here. Got them done last week! 🦋</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d79zuu</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1d79zjy</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Potion Polish Spring Set</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d79zjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1d79ygm</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>So I just found a bunch of polish I thought I lost and</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/63sm972t4e4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1d79ucf</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>The Rainbow Connection 🌈</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d79ucf</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1d79jms</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>My obsession with galaxy themed polish continues 🌌</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1jytltup1e4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1d794xt</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Nails match my cat’s inhaler lol</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d794xt</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1d78wo8</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Pride nails!!!</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d78wo8</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1d78pfo</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>Blue to Black Thermal</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sgyinhpovd4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1d78gyf</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>⋆˚✿˖° Flower ♡ Child ⋆˚✿˖°</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d78gyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1d77w6l</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d77w6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1d77uyr</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Currently chomping at the bit for the sequel being released tomorrow, but in the meantime here is a Butcher &amp; Blackbird themed mani that I loved doing! </t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d77uyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1d77in1</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>The best brand for purples?</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d77in1/the_best_brand_for_purples/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1d76pva</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Orly polish</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d76pva/orly_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1d76mf1</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Oh, y’all thought I was done doing Pride themed nails? Nah, not even close. 🏳️‍🌈🌈</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d76mf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1d760ie</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>What to ask to the nail technician for an iridescent or pearly nail look?</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d760ie/what_to_ask_to_the_nail_technician_for_an/</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1d75up2</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>I am still obsessed with this collection</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d75up2</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1d74n5x</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>cake day nails 💜</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d74n5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1d74678</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>ISO dupe of Lumen Morpho Glow!</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d74678/iso_dupe_of_lumen_morpho_glow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1d73ztu</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>happy pride month! 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d73ztu</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1d73z33</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Reflective magic ✨</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d73z33</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1d73xxg</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Gamma Ray Blaster</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d73xxg</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1d734qw</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Holo Royalty Shimmering Secrets</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/inrom9rxnc4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1d72m8m</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Favorite manicure</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d72m8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1d725co</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>Death Valley Nails- Swamp Sparrow ❤️</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d725co</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1d70t44</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d70t44/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1d6nd1m</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>CND Shellac Top Coat</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d6nd1m/cnd_shellac_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1d6qydt</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>🍊🦖 bluebells and monsters 🦖🍊</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d6qydt</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1d6x51m</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy pride! </t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uhd5bxevma4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1d7qios</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>What should i get done at the nail salon ( the pictures I’m showing are not my pictures they are pictures I found on Pinterest)</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7qios</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1d7q29y</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Happy Pride! 🌈</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0u9brvszvh4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1d7po52</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Various nail designs credit: @aniisafar on ins
+Artist:https://www.instagram.com/aniisafar/</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b4heo6cvqh4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1d7oh9t</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>New</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/saphyh0feh4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1d7m67p</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Floral 🌸 </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7m67p</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1d7l999</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>rave ready?</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bfqvkvqjg4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1d7jluz</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Splendid little stars nails by nassa nails Ig</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxcz5nbn4g4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1d7hjpq</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Magnet suggestions</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1d7hjpq/magnet_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1d7h5vk</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>I continue practicing, what do you think? I love almonds</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tpl86gdtkf4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1d7fw3v</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Did my friends nails</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7fw3v</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1d7fqau</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>The Nails Bae Airbrush set. What you guys think? IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwp8b7kz9f4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1d7erka</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>💚🍏</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7erka</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1d7e93c</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Clear / White Marble for Summer</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cq1mciccze4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1d7bpz5</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Jeweled beetle nail art 🪲💅🏻 credit: @davids_nails</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsk0vgbhhe4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1d77tbv</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Just did these today. What you Think? IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/arw3j3qapd4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1d70lwm</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Summer Inspo</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/44s6omg2wb4d1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jun  5 08:08:51 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_09.xlsx
+++ b/data/2024_06_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C477"/>
+  <dimension ref="A1:C647"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8545,6 +8545,2896 @@
         </is>
       </c>
     </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1d8k66a</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying to regrow my nails after depression </t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/famovxv5ip4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1d8ju6g</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Cloudy with a chance of Lavender ♥️</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tdvg3ehrdp4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1d8je0i</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Love this color 💙</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otx2qt968p4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1d8jbvb</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Fruit nails for summer</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8jbvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1d8j1t1</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Natural</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v7bfh4dy3p4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1d8j0xq</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>I was iffy about this blue but ended up LOVING it. 🩵</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6h2lson3p4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1d8inye</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does gel glue leave behind indent or do I need to soak more? </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8inye</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1d8hun2</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>My boyfriend said this set was "low-key" 😂</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8hun2</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1d8hepm</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm a perfectionist and it takes me hours to do nails </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d8hepm/im_a_perfectionist_and_it_takes_me_hours_to_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1d8hfoq</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>My 3rd set of nails!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8hfoq</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1d8hbce</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>In love with this set i just did</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8hbce</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1d8h940</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>For those who do nails for a living..</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d8h940/for_those_who_do_nails_for_a_living/</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1d8gv66</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>my first time doing gel-x vs. my third time!! 😭</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8gv66</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1d8grc9</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>neon for pride month !!🌈🌈🌈🌈🌈🌈</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8grc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1d8gni0</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Did gel for the first time!!</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8gni0</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1d8ggjp</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Rubber gel has changed my life!</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xu5efg1vbo4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1d8g9lz</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Some advice and help</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d8g9lz/some_advice_and_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1d8fdiy</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>ATTENTION ALL GEL GIRLIES: I have some questions and curiosities! Can you help?</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8fdiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1d8fge9</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>My nail glue turned white?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jzqu1xb22o4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1d8g6uc</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>My fiancee did my nails</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8g6uc</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1d8ftod</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dark green 💚 </t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gw0b8ail5o4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1d8fqf8</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Sun moon and stars</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8fqf8</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1d8fiyh</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Natural nails</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8fiyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1d8famy</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Attempted painting some nail art by hand for the first time today</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q450ivfk0o4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1d8f6pi</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Loving my marble nails</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/udwmyj9kzn4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1d8f4tf</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Yay or nay?</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8f4tf</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1d8ejjr</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>Unhappy Customer</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8ejjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1d8dxjc</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>What's your favorite shape and length?</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d8dxjc/whats_your_favorite_shape_and_length/</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1d8dqnm</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Strawberry milk cow 🐮🍓</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rmcf419mn4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1d8dne2</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Press ons for graduation</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8dne2</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1d8deau</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Love a classic white nail moment 💅🏼🤍</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuq2o009jn4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1d8d8i2</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails buffed with a nail buffer Vs Japanese manicure. Zoom in to take a good look. </t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gcb96w4thn4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1d8cuib</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>help choosing colours for my mam</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rzpq6w6gen4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1d8cxz5</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Happy Pride🌈</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/puuh9bx9fn4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1d7vild</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about acrylic </t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7vild/question_about_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1d86ho2</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Dip + BIAB on top?? (Allergies)</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d86ho2</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1d8clia</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How much should these be? </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q4p5dns8cn4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1d8cjta</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>Natural but make it cat ✨</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fa69li4ubn4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1d8burw</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Top coat keeps coming off and idk why</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e3tbfiz16n4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1d8buea</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>If my fingers can’t be mistaken for highlighters, I don’t want it 😤🪸</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8buea</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1d8bsat</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>It’s been [0] days since a company accident.</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8bsat</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1d7l75a</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>Should I try to teach myself Gel-X or acrylics?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7l75a/should_i_try_to_teach_myself_gelx_or_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1d8b2ib</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>How do I get this brush/nail glue off this surface…? Soaked in remover a few times…</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kx491htnzm4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1d8bfgb</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Dip powder nails</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y9sz0ivj2n4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1d8b3cq</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Got my nails done today and I love them 💚</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ij1w04kuzm4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1d8b293</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>Any Jujutsu Kaisen fans here?</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0o9ev6qlzm4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1d8avxl</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>New colour.</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8avxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1d8ao3p</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Pressies are so fun</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8ao3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1d8adr2</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>I spent 20 hours on these</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8adr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1d7iacp</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Mani for my cousin’s quinceañera!</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7iacp</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1d7j59x</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>What is “Liquid Gel”?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7j59x/what_is_liquid_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1d7j7hx</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>been trying my hand at nail art recently so here's a les mis inspired set!</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7j7hx</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1d8a75y</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>These might not be for everybody but I’m in love</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bq6zo5nysm4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1d89zpd</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>What is the best tool to get rid of hangnails?</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d89zpd/what_is_the_best_tool_to_get_rid_of_hangnails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1d89vp1</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Go Oilers! 💙🧡🏒</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hszo3axfqm4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1d89rpx</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>My latest babies!</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fu18vsnnpm4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1d89h2i</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Piet Mondrian inspired mani</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d89h2i</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1d7pcvv</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Gel nails keep deattaching</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1r8ffoh0oh4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1d7r4pg</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>would a nail salon do one nail for me</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d7r4pg/would_a_nail_salon_do_one_nail_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1d89fyy</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>Is it normal for hard gel refill to cost nearly the same as the original overlay?</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d89fyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1d80gx1</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>If I volunteer, should I get a budget practice hand or use spare press ons for learning art and and regular polish (and gels on myself)? Are there universal standard practice hand and nail sizes and materials?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d80gx1/if_i_volunteer_should_i_get_a_budget_practice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1d84fiw</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Is there a way to know which Top Coats are compatible with which Polishes?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d84fiw/is_there_a_way_to_know_which_top_coats_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1d8955n</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Bluebell</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8955n</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1d7ix0c</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>My pride month nails! (Inspired by nailsbycarmen1310 on TikTok)</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7ix0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1d7n0to</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>If I could permanently have my nails like this I would!!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7n0to</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1d7uv43</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>I have a blank canvas and need some inspo</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvh30erbjj4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1d7wka3</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Here are some of my past nail designs. Which one do you like?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7wka3</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1d86w9t</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>White circles ⚪⚪</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1wlnitj4m4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1d82zr1</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>How do you like these?</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1pszsexbl4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1d88r9g</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Melanie Concert Nails!!</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d88r9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1d86r0g</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>what is up with this type of nails</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d86r0g</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1d86yzx</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>🌈🌈 set</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9i8dd5l35m4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1d88ps0</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>That one time I actually got my nails done in the salon</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8i6oe9qrhm4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1d88ngs</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>My nail tech is so awesome</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d88ngs</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1d88mzk</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone bring their own tools to the salon? </t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d88mzk/does_anyone_bring_their_own_tools_to_the_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1d87szk</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What can I do to make these better? </t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d87szk</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1d876yh</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic set I did today! </t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d876yh</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1d88gr9</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite summer polish </t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ame3ei8yfm4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1d889z2</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Jelly Nails</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3nf3aw4jem4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1d87re0</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Thick top coat recs?</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d87re0/thick_top_coat_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1d87gb5</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>I’ve only had this set for three days and I’ve already gotten so many compliments on them!</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d87gb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1d86zeq</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Splash of color! 🌈</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ik6hn0b65m4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1d86yqu</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>I think my nails have stopped growing</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d86yqu/i_think_my_nails_have_stopped_growing/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1d86xui</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving these strawberries 🍓 😍 </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7eunefv4m4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1d86tnv</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>1/4 Nails</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycevb6c04m4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1d86hp3</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Proud of my lil cherry French nails 🍒</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d86hp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1d86f2a</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Fun &amp; fruity for Pride (get it) 🍓🍊🍋🍉🫐</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hqnit4h41m4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1d8661p</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Cow print has become my fav</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8661p</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1d865xv</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Vertical lines one my nails</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d865xv</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1d85t45</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Got my nails doneee</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d85t45</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1d85hrv</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some cat eye love </t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d85hrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1d8578t</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Is it my nails or the fake nails?</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8578t</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1d853xh</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Opi malaga wine dupe?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d853xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1d84zls</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>What can I do to make these look better?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d84zls</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1d84uzn</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Are square nails a good shape for my hands? It never seems to look like reference pic</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d84uzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1d84nz5</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>I’m in love with the nails I got done today!! I originally wanted a pastel yellow but I love the retro vibes this color gives.</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d84nz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1d84cnu</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Hand painted Spongebob set on natural nails 🫧</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mfmv6e00ml4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1d848c7</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>this months nails🥰</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3w6ftkf4ll4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1d83yyj</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>What do you think? Do you like it? 💙</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pujlqqc8jl4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1d83uj9</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>How to make sure tips stay on my index</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d83uj9/how_to_make_sure_tips_stay_on_my_index/</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1d8k0ie</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Anyone use round nail swatches?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4fokcs0gp4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1d8iwfg</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Learning how to use my nail art tools</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3kjnx73y1p4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1d8io9q</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Honestly never expected to damage them in my sleep disappointed….</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6pqrf3jzo4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1d8gwwn</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>neons for pride month!🌈🌈🌈🌈</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8gwwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1d8g1pw</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple Strawberries 🍓 </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lir6ez5r7o4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1d8ff83</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>ATTENTION ALL GEL GIRLIES! I have some questions and curiosities! Can you help?!</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8ff83</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1d8f3wr</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>May 🌸</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8f3wr</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1d8eod3</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>I’m getting it!</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oze1yjksun4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1d8ej99</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>What the heck is this?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8ej99</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1d8d20d</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Rose &amp; Shine ✨ 💐</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8d20d</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1d8cnar</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Reporting unsafe products</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d8cnar/reporting_unsafe_products/</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1d8c8lf</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Fake Nail Envy?</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8c8lf</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1d8b3eb</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Cute little skit with bonus cursed poses</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8b3eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1d8ax9u</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BKL Ghost Walker vs Mooncat Petals For A Narcissist - swatch comparison available? </t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d8ax9u/bkl_ghost_walker_vs_mooncat_petals_for_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1d8awui</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New colour </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8awui</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1d8aad0</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>ORLY Bonder for chrome powder</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d8aad0/orly_bonder_for_chrome_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1d8a1ek</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Love is love</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8a1ek</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1d89zpz</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Dazzle Dry Coastal Cabana, a very close Tiffany blue match</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d89zpz</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1d89me1</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mesmerized by Merkitten </t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/081m0xhiom4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1d89a3h</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>ILNP Playlist 💚</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d89a3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1d894kv</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Mini mani day! My boys love joining me in this hobby. Here is my 6yo with some of his favorites.</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgu6od0ukm4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1d8928p</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Cinderella vibes ✨🩵</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8928p</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1d8917q</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>I don't usually wear polish this light</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cpywu35km4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1d890jh</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bluebell </t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d890jh</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1d88yth</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>💙</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wm29ejknjm4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1d88hr0</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>🌈 Nails</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/23d948e5gm4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1d88arf</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Jelly Polish </t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/do0uhpmpem4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1d87ibo</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>regular polish &amp; builder gel</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d87ibo/regular_polish_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1d86n57</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrome powder color/brand for red? </t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d86n57/chrome_powder_colorbrand_for_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1d86h3b</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Mooncat: Mercury in Retrograde</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h0ub9f1l1m4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1d85sup</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Full Scream Ahead and 1st official Mani-Mag test</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d85sup</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1d859b1</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>I love a layered moment with ILNP</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o65j0wxisl4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1d844gj</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t xml:space="preserve">😭😭😭😭 My bottle of Artemis's Deathkiss right before I was about to use it for the first time </t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d844gj</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1d843fv</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Atomic Polish</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d843fv/atomic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1d83x4h</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>BKL's Crimson Moth out in the wild</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d83x4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1d83iu5</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>More velvet, more butterflies!</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d83iu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1d830rk</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>New Mani - distracting me while I’m working!</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d830rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1d82lu8</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Ethereal - Moonbeam (PPU)</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2bjkgcld8l4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1d82lvn</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>RIP 🪦</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jckwfkf29l4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1d82lnt</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>ILNP -After Hours</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vavqa6o19l4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1d81y0f</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🌼 </t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d81y0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1d81nu4</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>This one exceeded my expectations!</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rhz74f12l4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1d81gta</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Love thermals.</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d81gta</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1d80ik4</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Can someone help me find dupes for these please?</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d80ik4</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1d804fd</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Shifty green and blue 💚💙</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d804fd</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1d7zsib</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>How do I make these look less chunky?</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7zsib</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1d7z7wl</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>The metro lighting makes bluebell look unreal</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iezufwg3kk4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1d7yre0</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not sure if I’m totally sold on the color but I feel like it’s giving old hollywood starlet vibes or something </t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7yre0</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1d7vaz1</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Disappointed with two Mooncat polishes from a third-party seller</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7vaz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1d7tjl7</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Orly - Artificial Orange</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7tjl7</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1d8im5h</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>is it obvious these are press ons?</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5fgzn7ouyo4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1d8g811</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>3D gel issues</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1d8g811/3d_gel_issues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1d8fk7t</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Some nail art samples with several themes! Personalized drawings</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8fk7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1d8e0xr</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>what are these type of nails called? I'm trying to get them done by myself but I can't find the name to look for the technique. Do they have a name? or are they done with gel?</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qwyvnm9son4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1d8cgwd</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These black nails are the best! Soft gel nails! </t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8cgwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1d8at9x</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>Sailor moon eyes hand drawn press on nails</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8at9x</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1d88g61</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Pride/Birthday Nails by Julie at Cozy Nails in Madison, WI</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d88g61</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1d87xr9</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Made some strawberry press on nails 🍓</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d87xr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1d877sw</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Acrylic set I did today! </t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d877sw</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1d84s56</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>I haven’t been able to take my eyes of my nails. This is the first time I went so short and this style is also a first. What do you think?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d84s56</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1d7yjp3</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>This is my first time painting on a nails</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7yjp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1d7ycmh</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>I’m in a committed relationship with my nail tech</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7ycmh</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1d7wemn</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Good morning! From Argentina</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7wemn</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1d7vxex</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Do you work with a pedicure? Good?</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6o1ip4gltj4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1d7vvee</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Good morning! A lot of love on these nails 💅</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7vvee</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1d7vfcl</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Black</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7vfcl</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1d7v1rn</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Good morning, we are already working! </t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d7v1rn</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1d7v13j</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Full 24 Set I Did For Someone </t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35r08w50lj4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1d7uus5</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>My wedding nails</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4ybs9j6jj4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1d7s8s5</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>My sushi nails</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fppt55q7ni4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jun  6 08:09:15 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_09.xlsx
+++ b/data/2024_06_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C647"/>
+  <dimension ref="A1:C826"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11435,6 +11435,3049 @@
         </is>
       </c>
     </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1d9d0s6</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Perfect red 💅</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9d0s6</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1d9cew6</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>A couple sets I made today 💕</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9cew6</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1d9cdcy</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time as a male letting my nails be done. </t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lriof5rvjw4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1d9caxz</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Avaca"toe" </t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t96hzuoxiw4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1d9bn13</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with this colour! </t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zav3j83paw4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1d9bm37</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Little summer moment. Been a journey to get my nails this long </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8f6b29xdaw4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1d9b5fk</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>I am in love with my cute summer nails 😍</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9b5fk</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1d986q9</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Why are my cuticles like this?</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rs3bgv69v4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1d9af5q</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>Having acrylics removed</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d9af5q/having_acrylics_removed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1d99x4l</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My engagement nails 💅 </t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2y2x804rv4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1d95bnn</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>SpongeBob Nails on a client</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d95bnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1d967vt</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>designs on short natural nails</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d967vt</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1d97d3n</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Recommend a cat eye magnet tool?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5t6xaff1v4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1d983o7</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Swipe to see where I started as a chronic nail biter… builder gel has changed my life!</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d983o7</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1d98g17</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>First time with 3D art! In Japan</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d98g17</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1d99cbl</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help ! </t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d99cbl/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1d98uv5</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>My 4 year old painted my nails</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f92v9brvfv4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1d98j6r</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Pretty pink💕💕</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d98j6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1d98hhd</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Want to start</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d98hhd/want_to_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1d98gry</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>First manicure ive done on someone else!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/20dzryuubv4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1d98b7u</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>✨ fun with Essie special effects ✨</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d98b7u</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1d984pi</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Getting the hang of the beauty shots</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d984pi</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1d97hj2</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>How can I cut my nail without ruining the polish?</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyr6v6mj2v4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1d97gyg</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>question about gel fill</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d97gyg/question_about_gel_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1d97ev5</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>Press on nail glue</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d97ev5/press_on_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1d97bm9</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail growth </t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5m1fqa421v4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1d974s3</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mother of pearl nails 🫧🦪⊹ . ݁ </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yywnw7tbzu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1d96l57</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Grad nails 😍</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d96l57</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1d96fzm</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Cuticles lifted after manicure</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4vvyprtsu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1d95tb2</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Sanrio Chococat custom nails, all hand painted by me</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/il1kbvr1nu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1d95qn2</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Did a little nail art practice!</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x513w9simu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1d95nh2</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>My nail text understood the assignment</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5t49amplu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1d95nek</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>I got a Wet N Wild gift set, all of the polishes are unnamed but i swatched them all</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d95nek</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1d95lfm</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Essie-Torquoise and caicos</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d95lfm</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1d95knl</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Bfs mom got me Sally Hansen-In A Blush</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d95knl</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1d958pj</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Pride Nails</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d958pj</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1d957o6</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>first time trying gel x (aprés)</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9nrwfsrhu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1d953cb</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>First time trying long nails!!</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d953cb</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1d94wv1</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Testing a new design</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6dwzq494fu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1d94sg5</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>🧿🧿🧿</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzkgxun1eu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1d94rlg</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>My short nails</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/53rhrc8wdu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1d94p8x</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Looking for advice to strengthen my nails for the next round of growth</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d94p8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1d94p62</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Natural nails 😫</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zmaz3tkbdu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1d94ng4</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Finally figured out my shape and how to manicure at home</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d94ng4</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1d94f3g</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>What do you think of these?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cb5v58xsau4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1d9445m</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>I think they turned out pretty well, inspired by the love hashira iykyk</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9dfn0p18u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1d94dzk</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>You are nails in soft gel. They drove me crazy! I love the cat's eye effect.</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u10z9v2jau4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1d949eb</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Are gel nails suitable for people who work with their hands?</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d949eb/are_gel_nails_suitable_for_people_who_work_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1d942lk</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Nails are ready for vacay 🏝️☀️</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d942lk</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1d940kx</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>Did these Gel x for a friend!</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d940kx</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1d93y2x</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Red stilettos</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8oz746ko6u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1d8m44q</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>Can someone tell me what's wrong with my nails? 😭</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6mzlsl17q4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1d93wq5</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Second Time Doing My Nails On My Own</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d93wq5</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1d93v4n</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Saving Money</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d93v4n/saving_money/</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1d93uhx</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>french pink</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/SQuhVC1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1d8y4ni</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Lost about nail care</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8y4ni</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1d93tjk</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>dragon eye nails</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d93tjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1d8yi4m</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>How do I stop this?</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8yi4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1d919n7</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails inspired by Turkish Evil Eye 🧿 </t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d919n7</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1d93ph1</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>First aura effect (I think that’s what it’s called) what do you think?</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k476vn5p4u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1d93mfe</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>So in love with this starburst set</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d93mfe</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1d93kk5</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Party nails </t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5fdsxul3u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1d93fe2</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Summer Butterfly Nails</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d93fe2</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1d93cln</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Strawberry Nails</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mry7lg4s1u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1d93a9a</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Clase Azul Nails</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d93a9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1d9376p</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Buttercup nails</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9563555k0u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1d936gs</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>I got the bi flag colors for pride month 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d936gs</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1d92syu</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>How to protect lifted nail and prevent it from falling the rest of the way off?</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d92syu</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1d8z8q5</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Half way through bail school :)</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3qbhi3h6t4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1d9152i</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>🤍</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3krnh0fmkt4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1d90jpl</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Cat eye gel makes for the prettiest butterfly wings</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cmq13dg9gt4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1d90bw1</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>So happy with how this set turned out! 🤍🩷❤️</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d90bw1</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1d9063u</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cuticle oil post manicure </t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d9063u/cuticle_oil_post_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1d8zy89</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Squoval or almond? </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8zy89</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1d8z601</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>obsessed with swiftie set!!</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ule9xuww5t4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1d8yz84</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🌈 ✨ </t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8yz84</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1d8yt3d</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>What nail polish dries the fastest?</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w8lb39ba3t4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1d8yvak</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>Did a Gel X set on myself for the first time!!</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8yvak</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1d8yh2z</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Hand painted</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8yh2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1d8ydgg</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>Tips to improve nail bed?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8ydgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1d8xnvb</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>Is this a gel nail allergy or just irritation from removal/chemicals?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8xnvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1d8wsld</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Time Nail Art </t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d8wsld/first_time_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1d8wmy9</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>These Nails are the Bees Knees</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8wmy9</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1d8wcmf</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Forgot to post my current set</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbjuylhels4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1d8vppz</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>question about Russian manicure with gel extensions</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d8vppz/question_about_russian_manicure_with_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1d8vmhg</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>This set is titled: “The Morning After”: Builder Gel Overlay, was up until 2an making it this far. No cuticle oil, no polish… it’s the morning after. ;)</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8vmhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1d8v9wj</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Press ons by me</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qvt939tfds4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1d8v2rw</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>help!</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d8v2rw/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1d8ujwc</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Vivienne Westwood Inspired💖 🐊 💖</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sf96tm548s4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1d8ryff</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Can I get a pedicure if I have a janky toenail?</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d8ryff/can_i_get_a_pedicure_if_i_have_a_janky_toenail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1d8xx97</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>First Pride Nails of 2024</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixqdcpxtws4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1d8xs28</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>nails won’t last/ help 😭</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d8xs28/nails_wont_last_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1d8xqbk</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Summer nails with the bestie 🫶🏻 what do we think? 😇</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4pg87lggvs4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1d8xjmr</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Something simple for summer</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6fquyz2us4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1d8x7xq</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>First time making press ons 🌈</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5begocqors4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1d8x7ww</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>New nails, who dis?</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lv2yrbdnrs4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1d8x46h</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>option 1, 2 or 3?</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8x46h</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1d8wxy8</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>which shape?</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qy6813hnps4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1d8wxck</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Smileys 🙂</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ai96u1oips4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1d8wvam</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Summer jungle</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8wvam</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1d936ct</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>🩵 Polishes Used: Cirque Colors (Shade: Topsy Turvy) | Essie (Shade: Good To Go Top Coat)</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d936ct</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1d8tzc4</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>HELP ME ID these nails!!</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c1jp6b8u3s4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1d9btpk</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>where to buy emily de molly in europe?</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d9btpk/where_to_buy_emily_de_molly_in_europe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1d9a2ca</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>New to the polish world, nail tech destroyed my nails during filing for gel polish. Clarification for protecting them?</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d9a2ca/new_to_the_polish_world_nail_tech_destroyed_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1d96yc2</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>First Time Ordering from Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d96yc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1d96vul</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Fill today and silly questions from a newbie 🩶</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d96vul</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1d96pr8</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Polished for Days - Once Upon a Dream</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1eosox1evu4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1d96kvr</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Devil’s Ivy matches my hoodie 🥰</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l7cfi446uu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1d966lb</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>first atomic polish order!! 🩷🧡💚</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qs3q3bkqu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1d95zuq</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Rainbow in a bottle</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d95zuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1d95x8n</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t xml:space="preserve">✨ Nothing hits like that late afternoon bathroom lighting ✨ </t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/umck9ey6ou4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1d95215</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Enjoying my first order from Polish Pickup</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fb1ahjdgu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1d94n37</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t xml:space="preserve">“Drink the sea” is blurple perfection </t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d94n37</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1d94j8a</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>I love the color of Mooncat A Midsummer Night's Dream, but it's so hard to get a smooth finish. Any tips on minimizing bumps/bubbles?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t53qs7hubu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1d948jt</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Take me to your leader 👽</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qua7dde79u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1d940hr</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>It’s Only Forever</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d940hr</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1d93hrv</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>💙 Polishes Used: ILNP (Shade: Songbird) | Essie (Shade: Good To Go Topcoat)</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d93hrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1d93get</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>What a hot pink! Polishes Used: Cirque Colors (Shade: C’est Chic) | Essie (Shade: Good to Go Topcoat)</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d93get</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1d93eno</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>The holy grail of skittles 🌈 Polishes Used (Pinkie to Pointer): ILNP (Shade: Fairy Dust) | ILNP (Shade: Pixie Party) | ILNP (Shade: Flower Child) | ILNP (Shade: Bluebell) | Essie (Shade: Good To Go Topcoat)</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d93eno</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1d93ba5</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>I actually could not stop staring at this one 😍 Polishes Used: Cirque Colors (Shade: Dusky Skies) | Essie (Shade: Good To Go Top Coat)</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d93ba5</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1d938qs</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Graduation nails 👩🏻‍🎓 Polishes Used: ILNP (Shade: Melody) | Essie (Shade: Good To Go Top Coat)</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d938qs</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1d93767</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Maelstrom is beautiful and I can't stop staring </t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qack0fak0u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1d93348</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>anybody else get the ulta nail polish day gift(s)?</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d93348</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1d92ual</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>OPI for the win. Chopsticks and Stones with Essie no chip topcoat on natural nails.</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqbnsflpxt4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1d92ai2</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>This sub made me question how to best present my nails. So I wanted to give some options:</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d92ai2</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1d923ar</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>💙💛🧡🩵💚</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/776x2m0wrt4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1d90ltr</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to avoid allergies/polish reccomendations </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d90ltr/how_to_avoid_allergiespolish_reccomendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1d8yh7a</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PFD- Over the Moon 🌙 </t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8yh7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1d8y0q4</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>First Pride Nails of 2024!</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrnc80kjxs4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1d8x070</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail Polish Remover Pens </t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d8x070/nail_polish_remover_pens/</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1d8w9tx</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Would you buy press-ons with rare / discontinued polish colors?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d8w9tx/would_you_buy_pressons_with_rare_discontinued/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1d8w5t4</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Dark Omens 🌑</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0w6pqjxwis4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1d8vz89</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Best indie brands for warm tones?</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d8vz89/best_indie_brands_for_warm_tones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1d8vyna</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Moonicorn </t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8vyna</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1d8vmaw</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>They're not the same! (No seriously, only vaguely similar...)</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8vmaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1d8vcxq</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Who else is guilty of putting on a topper once your mani is grown out instead of repainting?😅 </t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8vcxq</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1d8unlr</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Bluetiful Blurple</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/pAiOwA9</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1d8un93</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>I NEED MORE MAGNETICS!</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d8un93/i_need_more_magnetics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1d8uau6</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>Year of the Dragon 🐉</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8uau6</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1d8tpuz</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>In LOVE with Whiskey Sunrise</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8tpuz</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1d8tncz</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Are regular polishes a risk with a gel nail allergy?</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d8tncz/are_regular_polishes_a_risk_with_a_gel_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1d8t6k7</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail polish thinner evaporating </t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d8t6k7/nail_polish_thinner_evaporating/</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1d8t5bi</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Another side of Bluebell</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rpy5jpukxr4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1d8smy7</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>🎶Sparkle doo doo doo doo doo, Oh flakie, flakie 🎶</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8smy7</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1d8s41w</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Gifted oil, could I use as a nail oil?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imguoajupr4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1d8rx42</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>ILNP Tango from the Watercolor Collection</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8rx42</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1d8rqgc</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>What are some of the most unique nail polishes you own/have seen?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d8rqgc/what_are_some_of_the_most_unique_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1d8qsvi</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Find Me an Oasis (and some things that look like it)</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8qsvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1d8qldl</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Pink and Purple Mani</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx7qe7deer4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1d8qdzq</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>The nude of my dreams</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8qdzq</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1d8pft1</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>A Pain in the Asteroid</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fd0xhvas4r4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1d8nt3t</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My pride nails! </t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8nt3t</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1d8l305</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Advice on growth...</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/17hj7mi6up4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1d9ak4r</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Soy principiante. Les gusta?</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sp8gejb6yv4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1d9a2gz</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>Newest junk nail set :)</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9a2gz</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1d973a4</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Azules 🟦 amo este efecto! </t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d973a4</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1d971pm</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Good?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v9qqv77jyu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1d970e9</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Este efecto! 🤩</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kyobee17yu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1d96zai</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uñas naturalmente! </t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4aosilmwxu4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1d953tf</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>The most beautiful nails I’ve made, by myself!</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d953tf</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1d93ykq</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Black and gold nails</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plmof0bt6u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1d93nfo</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red stilettos </t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/boroibq74u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1d93lbb</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Buttercup nails</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4sly5wr3u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1d93c8r</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>French tip nails</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv266zvo1u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1d93b8a</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink sparkly nails </t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qooijpqg1u4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1d9015b</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Do you like it , With this design A little red today! Do you like it?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9015b</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1d8wdsh</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>The Simpsoooons do do do do</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l1qmx2zmls4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1d8v4rg</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Psychedelic nails for movement weekend in Detroit</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8v4rg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1d8tmkx</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Slytherin style</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8tmkx</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1d8tect</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>I look like a vampire.</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8tect</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1d8t6h7</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>A little color last week ✨</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8t6h7</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1d8t11g</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>delicate and beautiful</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8t11g</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1d8sx5r</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>love!</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8sx5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1d8sgpp</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>my friend did my nails</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eee0cc7hsr4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1d8sdyx</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>My Bridgerton inspired set patiently waiting for the next half of S3😅</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1a8lsawrr4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1d8rrqi</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Hydrangea and rain drops</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8rrqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1d8pk93</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>absolutely marrying my nail tech @dani_thenaildon 📍 Hoboken, nj</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jgat78rw5r4d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1d8mjh5</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>I would like a specific colour in my home salon</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1d8mjh5/i_would_like_a_specific_colour_in_my_home_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1d8kpau</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>This packaging feels full of sincerity; I'm planning to give it to my friend as a birthday gift next week 😊💅🎁</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d8kpau</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jun  7 08:09:16 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_09.xlsx
+++ b/data/2024_06_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C826"/>
+  <dimension ref="A1:C1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14478,6 +14478,2998 @@
         </is>
       </c>
     </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1da4s90</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>I'm obsessed</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1da4s90/im_obsessed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1da4lnf</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>First time having done my nails</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da4lnf</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1da454h</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thank you all for your support and suggestions on that post. I also realize that the title of that post was inappropriate. I bought that nail art from a niche brand, so I felt that the style was quite niche, which led to a title that many found off-putting. I sincerely apologize for this. </t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da454h</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1da3plw</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Different than most girls</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1da3plw/different_than_most_girls/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1da3e05</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Help. Do you tip for a manicure done in their home?</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1da3e05/help_do_you_tip_for_a_manicure_done_in_their_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1da39o5</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>✨ Glamour Magick ✨</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7oz2any635d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1da2lke</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>Which nail shape suits me best?</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da2lke</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1da2291</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>New birthday set</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/52opqk4vt25d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1da1l2n</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>Second Attempt of Press Ons</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da1l2n</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1da1ehj</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Lemons for summer 🍋</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/csz5lj0zm25d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1da1avf</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Simple gurrrl</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0aqe6j4xl25d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1da15ae</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>My favorite ✨red✨</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da15ae</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1da0yzo</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>I decided to paint some lettering on my nails</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da0yzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1da0wqw</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>nails for a jalisco vacation 💙</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d2qydpszh25d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1da0613</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>My favorite way to do nails</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da0613</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1d9zxin</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3rd attempt </t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9zxin</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1d9zrh9</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>had a girls day and got our nails done 🥰</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mnt98gp6725d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1d9zq9l</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - Yetti to Party - Ügly Xmas Sweater Advent '23</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9zq9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1d9zmse</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>My third time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx3312cy525d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1d9zkfh</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>What u got vs what I ask for</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9zkfh</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1d9zgep</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>bday set🪽</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ogob2z8a425d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1d9z9xi</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>would you let me do your nails?</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f6u2f6cm225d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1d9z6ng</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Moon Cat in Ghost of Hecate.</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q1bvysbs125d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1d9z4ui</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>My nail tech let me try on her ring and I need to show more people!</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jvzkf97c125d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1d9z3zj</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>💗🎀💅🏼</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qhduvz94125d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1d9y37c</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>I’m in Love with these 💅🏼</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/czlf2yqpr15d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1d9xted</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Hello Kitty nail art 🎀</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9xted</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1d9xnoy</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>I’m OBSESSED</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9xnoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1d9xlgf</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pregunta </t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d9xlgf/pregunta/</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1d9xg3x</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>my favourite set yet</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9xg3x</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1d9xep2</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>hawt girl nails</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9xep2</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1d9xbat</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Paint set</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ddodiugqk15d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1d9xbvx</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>most recent set!! (HEAVILY inspired by pinterest, last pic)</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9xbvx</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1d9x930</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Got charms for the first time, I like them</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9x930</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1d9x92q</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>my first ever time using chrome!!!</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9x92q</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1d9x8b4</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Some of my press on work 🖤</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9x8b4</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1d9x1wr</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Twinning with my favorite sticker </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmcr8lgki15d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1d9ilbm</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>How do I keep my nails from snagging?</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d9ilbm/how_do_i_keep_my_nails_from_snagging/</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1d9j3f9</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>How do I save money but still have nice nails?</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d9j3f9/how_do_i_save_money_but_still_have_nice_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1d9wzpm</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍑 movin to the country gonna eat a lot of peaches </t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h150ri42i15d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1d9wxbx</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>almond blue</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/MC7xecz.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1d9wqcf</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t xml:space="preserve">it's the neon cherries for me </t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4r5s27uf15d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1d9wq1g</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>No face!</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49weucnrf15d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1d9we9e</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Cheers to being obsessed with my nails 💅</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9we9e</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1d9wcya</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Need advice: How to DIY fix the wide, thick awkward tips on my chrome manicure</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9wcya</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1d9w7lh</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Pride nail!</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bb901hwgb15d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1d9w6gr</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dum dum wrapper first time trying this ! </t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfv60eg7b15d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1d9vy8l</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ypsra4e915d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1d9vsrk</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>can i remove cuticles if i have on fake nails?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d9vsrk/can_i_remove_cuticles_if_i_have_on_fake_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1d9vmpc</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>How long of cutting this part back until it naturally grows in smaller/non existent</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9vmpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1d9v9rz</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Redid one of my fav designs from last year! 💚🔐</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9v9rz</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1d9v2ag</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>My prom is in 6 days - how can I fix my nail?</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojv9pxq8215d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1d9ulye</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>About this pink</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9ulye</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1d9uiij</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Nonbinary Sanrio nails for pride month!</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9uiij</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1d9uf39</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>What is better Acrylic nails or gel to work with?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d9uf39/what_is_better_acrylic_nails_or_gel_to_work_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1d9tutb</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Asked my nail tech for strawberries and flowers!</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3q1i70eys05d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1d9tqzu</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Don't think I'll ever get tired of french nails</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9tqzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1d9tbb6</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>Rate my nails?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bbk9np21p05d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1d9t29z</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Gilded nails, just messing around</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9t29z</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1d9t16t</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Nails i did on myself as a semi beginner!</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8h69g30n05d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1d9sq3a</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>Fresh acrylics for my vacation</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jr5odp9rk05d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1d9smzr</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Floral nails I did</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9smzr</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1d9sgf6</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Before and after care. Buff and shape</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9sgf6</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1d9k038</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>Weak nails after dip?</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d9k038/weak_nails_after_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1d9l9ds</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Light pink and gold flake</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3aif10js1z4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1d9sbom</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying out almond nails! </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9sbom</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1d9sa8m</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Clean girl nails</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/img208vjh05d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1d9n9ty</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Rings of Fire - Can I still get a fill?</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d9n9ty/rings_of_fire_can_i_still_get_a_fill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1d9mbgk</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>any way to prevent this nail from more damage?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hoprpxm9z4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1d9rf90</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>is it time to move on from my nail tech?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/naad60eab05d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1d9qxk1</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Vanilla Chrome ✨️</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9qxk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1d9qkfq</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My wife and my nail polish. </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4iswcaj7505d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1d9qgui</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Long practice nails!</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9qgui</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1d9qca4</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>The tiniest gel manicure I’ve done</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5svlpt1k305d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1d9q5xv</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help! Bleeding after pedicures </t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1d9q5xv/help_bleeding_after_pedicures/</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1d9prdl</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Cat eye claws</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jotv8fqazz4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1d9pzjr</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>paid $50 for this.</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9pzjr</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1d9p6t4</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>I think I am different from most girls.😕</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9p6t4</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1d9pxqu</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>kuromi nails^_^</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bkwrwpm005d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1d9ph0f</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>My mom bought a dip kit and hated it, she gave it to me to try and I love it</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9ph0f</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1d9p7gy</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>French with shiny nail powder 🤍✨</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0k94aaw6vz4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1d9olqz</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Rose/ nude</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sldf5yeqqz4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1d9oks6</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>How much would you pay?</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9oks6</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1d9odip</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing the dip powder. I was proficient in acrylic and had just learned gel enhancements when this stuff hit the market years ago. I regret not trying this sooner! Soooooo much easier! </t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9odip</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1d9o1i0</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>When your nails match your snack</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9o1i0</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1d9nihh</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Reach for the stars ✨🌟</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9nihh</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1d9n551</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Polish color</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mx5qhaqufz4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1d9mrwa</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>My Bridgerton-inspired nails! 🎀🎻💅</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/br8oxlu1dz4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1d9lnfh</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Nail suggestions that match this dress!</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ajtxazr4z4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1d9ln76</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Need nail lamp suggestions for beginner</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9ln76</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1d9lb4g</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>3d flower set 🌸💅🏼</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9lb4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1d9kypx</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Summer Nails 💜💛</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9kypx</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1d9kmir</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Orange flow for grad 💛</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqvv3ac0xy4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1d9k4go</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Saw a cherry on the ground my nails are the same color 🍒💅🏻</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eg125vacty4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1d9j77h</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Obsessed with these!!</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9j77h</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1d9ixgd</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Loving the Cat Eye French Tips</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uizfevv3ky4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1d9i09l</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Pride press one</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8c97eo5mcy4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1d9hfz3</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Tips and advice with white polishes!</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9hfz3</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1d9h62s</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Back from travels with magnetic green🌿🌱</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9h62s</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1d9h19l</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>clear set!</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzxut2qt3y4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1da525m</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Looking for nail polish dupe: innisfree #251 Grape Shake</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da525m</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1da32ga</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>I don't buy backups to keep my collection "moving," but some polishes make me wish I did 🥲</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x35i7bbr435d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1da2vyo</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Rainbow Pride Mani 🌈💅</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da2vyo</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1da2fd2</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Looking for polish recs</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1da2fd2/looking_for_polish_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1da19pr</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>This polish is a beautiful pain in the ass</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vfcet31ll25d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1da0tb2</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkles ✨✨ (NSFW for swearing) </t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y97xc202h25d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1da01rh</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Newbie but it's giving shego</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da01rh</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1d9zpik</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>Mooncat polish opinions</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d9zpik/mooncat_polish_opinions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1d9znz8</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer - Yetti to Party - Ugly Xmas Sweater Advent '23</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9znz8</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1d9u27a</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Obsessed with this unknown gel polish, can you help me identify it? So glowy!</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d9u27a/obsessed_with_this_unknown_gel_polish_can_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1d9y2ob</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Found this underneath two bottles of nail polish I got from dollar tree</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gp62qslr15d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1d9xhr9</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Natural vs indoor light on today’s mani</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9xhr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1d9x46s</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Polish Thinner</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehbwjca2j15d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1d9wlqb</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Changed it up with short nails 💚💙</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9wlqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1d9weom</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>OPI Glazed N’ Amused skittle</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jigj6ag3d15d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1d9w92i</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>Milky Stars ⭐️ 🥛 ⭐️</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9w92i</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1d9w8s8</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Gelcare Le Manouir brand damage</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d9w8s8/gelcare_le_manouir_brand_damage/</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1d9vlm4</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Any tips for destashing when you're a simple-minded dragon lady who guards a hoard of shiny things?</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9vlm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1d9v0ul</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>BKL Minora (Heartless Hunter): does it exist?</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d9v0ul/bkl_minora_heartless_hunter_does_it_exist/</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1d9uxzu</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Russian manicure chipping at 2wks, what's next?</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxo0av8a115d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1d9ue1s</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>We have "Maelstrom" at home...</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2b9j4t0x05d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1d9tgd7</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Alien/Outer Space theme 👽🛸🚀</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9tgd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1d9qy78</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Storage solutions for large collections? </t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d9qy78/storage_solutions_for_large_collections/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1d9qqzu</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>In desperate need of nail REHABILITATION</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9qqzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1d9q2fw</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>I guess it isn't *everything* I fear</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9q2fw</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1d9puoj</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Press on nail recommendations?</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d9puoj/press_on_nail_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1d9pn0h</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>ILNP - deep space</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9pn0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1d9phm9</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Polka Dot 💛🧡🩷❤️💜💙🩵💚</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9phm9</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1d9ph2x</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>French with shiny nail powder 🤍✨</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfwptoz7xz4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1d9pesm</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Loving this combo!</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tl9v8b6rwz4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1d9oiu5</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Cute Cat Inspo</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9oiu5</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1d9odum</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>How do you all organize your polish? By color or brand?</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/otwsc8x4pz4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1d9o4rk</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Gel Nails Keep Peeling Off</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9o4rk</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1d9lvqy</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>🥤Diet Coke🥤</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9lvqy</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1d9lnex</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>ILNP poison velvet nails😍🩸</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kwmbobqr4z4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1d9k6tn</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Best red glitter polish ?</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1d9k6tn/best_red_glitter_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1d9j49y</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Phoenix - Lullaby</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9j49y</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1d9iz6x</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>My new favorite nail shape and color</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dxmkq9lhky4d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1d9gzgj</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>80s fluro nails</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bl46q01c3y4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1d9gvnc</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Be gay do crimes...but don't break a nail</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9gvnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1d9fmld</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>New summer mani!</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wn88pprlpx4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1d9dtrp</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Bi nails 🩷💜💙</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i50xq9il3x4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1d9d6mb</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Thank you to u/prettypurplepolishes for posting the MoYou London sale. I really didn't like how this originally looked but the stamps added that 'something missing' I was after! I know they're very messy but first time using a stamper and stickers 🙈</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9d6mb</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1da0gat</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>♥️♥️  que les parece este diseño!</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/70ofquzod25d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1da025s</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Les dejo este hermoso Capping en polygel </t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da025s</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1da01k0</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Verde oliva 🫒  les gusta?</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xvgg8crs925d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1da00x3</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French! </t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5u2tm4wm925d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1da00d1</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Almond nails!</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lngqdz9i925d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1d9zzdx</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>antes y después 🤩</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9zzdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1d9zyo5</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Uñas soft gel ! </t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9zyo5</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1d9zxwp</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Good?</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9zxwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1d9zgt5</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Photoshoot nailz🧚🏻‍♀️💌💅</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9zgt5</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1d9zb7u</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Ice cream ☀️</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/76rlweiy225d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1d9yfs2</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Hand painted nail art by me.</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wukl49lvu15d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1d9y388</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>Last weeks leopard set 💜🖤</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9y388</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1d9xra4</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Hello Kitty inspired nails 🎀</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9xra4</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1d9xcwy</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Not the typical summer nails..</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l8a0rsd3l15d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1d9wgo5</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you get chrome to only stick to some parts? </t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1d9wgo5/how_do_you_get_chrome_to_only_stick_to_some_parts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1d9w97g</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pride nail! </t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gwove6wtb15d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1d9u888</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>The Nails Bae Marble Gold Chrome Set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9u888</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1d9tnn7</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Is it obvious that these are press ons?</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9tnn7</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1d9tgmf</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Just started creating nail art two days ago, made these while practicing 💕</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9tgmf</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1d9qlsc</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Teal and neon pink (DIY press ons)</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9qlsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1d9pjok</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mh5157uqxz4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1d9p9gq</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Trippy nails for Khruangbin show</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9p9gq</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1d9mah7</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Is it too simple? What do you think?</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/56hvizmb9z4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1d9l8jz</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>The Insect Chronicle in Nail Art! 🐞💅</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9l8jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1d9kjqq</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>new to gel nails!</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9kjqq</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1d9kdd4</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Which butterfly nail design would you choose? 🦋💅</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9kdd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1d9k4ep</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>I try to take most of the photos during the day but it’s been gloomy in LA💖</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9k4ep</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1d9jn7l</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Pink nails</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k243xhllpy4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1d9jav6</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Just saw this post about the blue butterfly nail art, and I feel that my butterfly nail art is eclipsed. I really like this kind of packaging. 😮🥰</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9jav6</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1d9iufu</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9iufu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1d9ievr</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>Have to let my nails outgrow, so I chose this half and half design.</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9ievr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1d9hs87</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Gel X nails for myself</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mdncgcopay4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1d9go1q</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>First Atempt</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7s1n2f9a0y4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jun  8 08:07:59 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_09.xlsx
+++ b/data/2024_06_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1002"/>
+  <dimension ref="A1:C1172"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -17470,6 +17470,2896 @@
         </is>
       </c>
     </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1dawsn9</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Press on convert</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/td0fczwsoa5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1dawfy6</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>First time getting stick-on nails:)</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dawfy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1daw53b</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Which shape is best?</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daw53b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1datwb7</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Advice for home supplies</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1datwb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1dasp04</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Help for a Newbie</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dasp04</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1dabpf2</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Advice pls</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dabpf2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1dab8g2</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Best Gel Nail Polish</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dab8g2/best_gel_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1daa1br</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Nail extensions and nail health</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1daa1br/nail_extensions_and_nail_health/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1da5azs</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basecoat w/ uv filter? </t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1da5azs/basecoat_w_uv_filter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1davsye</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>my current set :)</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q8rund54da5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1davp7t</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>clase azul inspired nails i did on myself!</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4um85ylvba5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1davhwp</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Growth is mine, a bit of "no" colour to rest on 🩷</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o47evxni9a5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1davc3p</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>I'm still a beginner with nail art and I want to know if I'm on the right path.</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1davc3p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1daur2o</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>What shape suit me best do you think? What colors?</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daur2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1dauemt</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Rubber base seems "rubbery"</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dauemt/rubber_base_seems_rubbery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1dauc41</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>My wife has the best nail designer tho</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dauc41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1datyc2</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>New nails I did yesterday. Matte mildly transparent white with solid white accents. Only took 4 hours but proud of me😌</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1datyc2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1datob1</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Simple Set 💞</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1datob1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1dat35v</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>fun florals!!</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0vx6h699k95d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1dasqwp</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Full set of the Koi fish</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dasqwp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1dasl6t</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Advice for a newbie please</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dasl6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1daryf5</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>First time doing press-on nails</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daryf5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1dar76s</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t xml:space="preserve">French using dip powder </t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dar76s/french_using_dip_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1dar1hf</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Wallpaper Themed Nails</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dar1hf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1daqobh</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Wanted to share this set here one more time with better lighting 🩷</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pv9nkam0x85d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1daqey9</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Tried something different today</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daqey9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1daq90y</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Loving this red for summer ☀️</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daq90y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1daoibq</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>Giving my natural nails a break + nail stickers</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daoibq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1dapxxe</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>first time doing french pedicure on myself and it’s a vibe</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/od1xgdo7q85d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1daptbz</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it normal to soak after nail tech has painted gel nails for pedicure? </t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1daptbz/is_it_normal_to_soak_after_nail_tech_has_painted/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1dapegh</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Recommendations?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dapegh/recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1dapdh7</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Love this color from Mooncat!</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24q365qbl85d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1daol0n</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My best friend does her own nails and she's seriously amazing at them to me. These are dip some builder gel and then sometimes she will use btartbox glue on for if her nails if decide to betray her. </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daol0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1dao6fc</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>favorite nails over the years 🤌</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dao6fc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1dao6re</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ACOTR Night Court Nails </t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dao6re</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1dao2cu</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>obsessed :)</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dao2cu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1danqza</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>Dip Powder with Gel and UV Lamp?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1danqza/dip_powder_with_gel_and_uv_lamp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1danjnp</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Textured aqua chrome nails </t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1danjnp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1danb1b</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>Can you mix and match nails and gel?</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1danb1b/can_you_mix_and_match_nails_and_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1dan9xj</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>My first time making press on nails. Any tips?</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dan9xj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1dan9s2</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>My favorite time of the month!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dan9s2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1dan4xs</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Gel polish on acrylic overlay xx</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ydiqfgp0385d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1damu5r</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>What do you think of these designs?</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1damu5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1damsya</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Mani/Pedi ideas for 50’s car show</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1damsya/manipedi_ideas_for_50s_car_show/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1damon0</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>help! scuffed dip-powder nail</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mhhvnnujz75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1damo0y</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>New Chrome Nails</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1damo0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1damn81</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Press Ons too Big?</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1damn81</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1damn1r</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tropical 🏝️ </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dj7oary6z75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1daml7d</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>I’m gonna have to cut them 😭</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daml7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1damj9s</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Birthday settt</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vzf6mrj5y75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1damhkc</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>What is the best affordable gel x glue?</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1damhkc/what_is_the_best_affordable_gel_x_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1dalr4j</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>🍊 ‧₊˚ nails 🌺 .𖥔 ݁ ˖</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dalr4j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1dalkmc</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>new set 😝</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dalkmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1daldkm</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Sonny Angel Inspired 🤡</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t8qksho8p75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1dalcxm</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>🧡 Ella+Mila Mango Pop and Ninth St 🎈🎉</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dalcxm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1dala0l</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>Favorite set I’ve done</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dala0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1dakwy2</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pretty pink daisies </t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tl1b8y0ul75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1dakwb0</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Head and feet in the ☁️'s 🩷</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4t05w2apl75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1dajr3s</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Colorful</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wt4t0548d75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1dajqlm</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Newww press ons</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dajqlm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1dajoq2</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>how do we feel on these for my next nails?</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sp7nwamqc75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1dajg7d</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Blue waves 🌊</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b1hr56jxa75d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1dajded</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you rate my work? My client wanted something in the style of vintage jewelry </t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dajded</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1daj48s</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lamps, gel and polish in Canada? </t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1daj48s/lamps_gel_and_polish_in_canada/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1d9zn5l</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Are these bad? My first time getting my nails done ever</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9zn5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1d9zihd</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Emotional Support Manicure</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1d9zihd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1daix5e</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Beach vacation here I come!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tv0wlf02775d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1dai9tn</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Rose Quartz Press-ons I Painted</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dai9tn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1dahvww</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>I love do this design in my nails</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pdii98pz65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1dahvtj</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>My go-to</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipiujijoz65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1dadrr1</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Whoever I do a fill, I can't help but appreciate the natural "before polish" look. This time I decided to rock it! </t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dadrr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1dafime</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | PPU - YouHooooo!!!</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dafime</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1dagrcb</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What’s the best way to heal natural nails? </t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dagrcb/whats_the_best_way_to_heal_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1daho6r</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Manucurist or Dazzle Dry?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daho6r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1dah98e</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>what do you think</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u542gnycv65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1dah17y</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Rate these black and whites</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dah17y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1dagqym</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Already messed pointer finger up this morning but still cute. OPI &amp; Morgan Taylor </t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dagqym</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1daglcm</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a few sets </t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sf9zzcuoq65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1dagl50</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>My nails with essence french manicure</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7gotmymq65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1dagh6a</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>holo cat-eye gel in the sun for pride month &lt;3</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yo351t1wp65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1dafxa9</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Bright pink for the summer 😍</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xe44x2ul65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1dabms7</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>What would you do differently?</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dabms7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1dafm53</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>would a nail salon do one nail for me</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8ga8dmlj65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1dafk35</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pearl nails </t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dafk35</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1daf3tx</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>Doing soft gel extensions at home. Can UV nail glue be cured using a LED/UV lamp?</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1daf3tx/doing_soft_gel_extensions_at_home_can_uv_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1daeso9</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>how much would you pay for this set?</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/omiw3oafd65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1daeha0</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tips for cuticles? </t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jblbde3b65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1dadzvu</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Did my own fake nails for the first time!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oqh1s3cj765d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1dadvyk</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Press ons for Graduation from Glamnetic!</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dadvyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1daderf</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Square or coffin shaped?</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daderf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1dade6i</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Is there anything I can do to repair this crack besides trimming? Both my thumb nails are cracked at the corner I think my nail bed is a bit weak right now.</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ft8fx094365d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1dadcyr</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Got my nails done for the first time yesterday. I really like how they turned out.</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dadcyr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1dadago</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye/magnetic category breakdown discussion </t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dadago/cat_eyemagnetic_category_breakdown_discussion/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1dad5la</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Any tips to make marble nails look less messy?</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dad5la</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1dacurk</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>These ~natural~ looking nails took me half a century to do. Feat. Goodest boi</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dacurk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1dacfta</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Is there any waterproof nail applicant? Protecting natural nails for constant hand washing?</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dacfta/is_there_any_waterproof_nail_applicant_protecting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1dabozo</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>My sister likes to practice on me. Princess nails this time 👑💎</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dabozo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1daan15</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>🧡</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daan15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1da9wbi</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>First cat eye set &amp; I’m obsessed!</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da9wbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1da9irb</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>🖤</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da9irb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1dasym6</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>Hot pink nails…perfect accent to go with a black &amp; white dress for a wedding!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8c1a79p0j95d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1darzex</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Matchy Matchcat 🌙💙</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1darzex</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1daq2ib</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Where should I start with my nails?</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daq2ib</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1daq1a2</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat A Midsummer’s Dream VS Aphrodisiac 🐈 </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daq1a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1dapw6l</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your favorite indie/boutique white polishes? </t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dapw6l/what_are_your_favorite_indieboutique_white/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1dapgaf</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Deeply obsessed with what’s going on here 💙</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dapgaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1dapau6</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Still loving my mooncat order!</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efrr837pk85d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1dapa93</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stamping polish? </t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dapa93/stamping_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1daoonr</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>Lumen - Glass Stars ⭐️</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daoonr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1danz4c</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>My nail broke badly</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kxhbql1n985d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1danrfd</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Holo Taco Collection boxes</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pozrtekx785d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1damw43</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>LEAST favorite polish??</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1damw43</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1daenli</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>FOMO Burnout and PPU</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1daenli/fomo_burnout_and_ppu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1daly5c</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Space cowboy dupe? </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1daly5c/space_cowboy_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1dalo36</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Whisper + Jade Jelly</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dalo36</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1dalmvz</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One hand has terrible nails, the other perfectly fine. What can I do? </t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dalmvz/one_hand_has_terrible_nails_the_other_perfectly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1dalbmd</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🧡 Ella+Mila Mango Pop and Ninth St. 🎈🎉 </t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dalbmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1dakmla</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Happy Pride Month! 🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wyt61ykqj75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1dak0sp</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>So juicy and sweet for summer!!</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cf9d9l1af75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1dajvco</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>SHIFTY</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dajvco</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1dajunx</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Peep these puppies</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dajunx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1dajt0e</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Essie Gel Couture question! Gel or regular polish?</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dajt0e/essie_gel_couture_question_gel_or_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1daji7y</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat addresses the bottle issue + offers to make it right </t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvx2gdmdb75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1dairy5</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What supplies do I need to make my own press ons? </t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dairy5/what_supplies_do_i_need_to_make_my_own_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1dair3n</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Time for sparkles! Orly bonder, INLP Madison Ave, Seche Vite</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3yp7xiq575d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1dailrd</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Shining, shimmering, splendid 🩵</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jhjhkwwt475d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1daifpe</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>I can definitely stand Lorraine</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daifpe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1dai6c8</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Rose Quartz Mani</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dai6c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1dahz5a</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Octo - Alien / Baroness X</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/76sf0oub075d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1dahnl3</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Peely base leaving residue</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dahnl3/peely_base_leaving_residue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1daglbj</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Love a good juicy jelly 😊🍉</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daglbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1dagl47</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>🍋‍🟩🍋‍🟩🍋‍🟩</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3d3lz1nq65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1dagfay</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Sassy Sauce “A Pain in the Asteroid”</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dagfay</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1dag3xx</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Newbie here! You all inspired me to try something new</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7n7ea016n65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1dafbgf</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Update: I had a chip, so I added some moar colors... Do you like???🫣🙈</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dafbgf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1daedyh</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Obsessed with Supervillain!</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ft1cx9xea65d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1dae4ag</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Is it normal for Cirque Lavender Sky to look like this?</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dae4ag</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1dadugy</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>What do you think? Which combo is your fav?</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dadugy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1dadgof</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Mooncat Siren’s Deceit</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dadgof</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1dad2oc</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Pan Pride nails for the pan babes out there. 💗💛💙</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dad2oc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1dac6kt</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I fix this? </t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dac6kt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1dabl7i</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>💙💚🤍🏳️‍🌈 MLM Pride Flag</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dabl7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1daadkt</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>How do you store your press on nails? Especially if you're in the EU, I can't seem to find good storage solutions (I do them myself, so they don't already come in a box)</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1daadkt/how_do_you_store_your_press_on_nails_especially/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1daa7da</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>Opi Nail Lacquer- color “Lima tell you about this color” Love this pink!</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daa7da</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1daa690</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not a Waste anymore </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daa690</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1daa4sz</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Tennis 🎾 ball color recs?</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1y1gq38ie55d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1da9z5a</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>I've found my perfect match: OPI Bare My Soul</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da9z5a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1da9tn8</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Absolutely cannot believe I slept on this one in favor of bluebell. Holy Flower Child magic! </t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2ynlvrnvb55d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1da9lxn</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Eras tour nails</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zwjekomy955d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1da7k98</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>✨ Starrily always gets magnetics right</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1da7k98</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1da6an6</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>For those of you who add an extra top coat layer a few days in, how do you prevent peeling and shrinkage?</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1da6an6/for_those_of_you_who_add_an_extra_top_coat_layer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1d9jwam</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>All of my cuticles are bleeding like this one after a manicure</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d0ojnxwkry4d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1daxpir</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails done in Vietnam </t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/my46t8z40b5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1daxlag</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">3rd ever nail art :3 I think I dis a pretty decent job! </t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1daxlag</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1dau14x</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Help on how to achieve this organic cloudy murky texture</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ajai1twnt95d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1davahc</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>First time 3D sculpting gel &amp; butterfly art !</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/onv7d6e47a5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1datq9n</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Working in my shaping and painting skills</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1datq9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1datao1</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Hi can someone tell me the name of this thing used for french chrome? (Can it be used for usual gel polish?)</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5x3ppn2am95d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1daruzg</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>How to Do Marble 3D Chrome Nails. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pltcp3z4895d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1dardpm</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some fun glitter and black </t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/paabaubm395d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1daqzc8</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These design is my Fav. Any advise for my nails? </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65odl593z85d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1dam38n</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>I love them💞</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dam38n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1dam277</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I painted my moms nails last night. First time I've done something other than a plain colour </t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p1wmy5afu75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1dam20f</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>First time doing my own nails at home 😅 still can’t get them to last without falling off though ☹️</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6capuc5eu75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1dallgf</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Don’t like it, idk why. Suggestions and CC?</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gx7hu9cxq75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1dakxxi</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Reptile</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p956ofa1m75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1dakvhx</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Little rainbow decals for June </t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n8o8pt2jl75d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1dakoh9</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>Stickers are my fav!</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dakoh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1dahdhb</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Miren este crecimiento! </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dahdhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1dacala</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Guy looking for advice </t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cdq7deyu55d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jun  9 08:07:58 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_06_09.xlsx
+++ b/data/2024_06_09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1172"/>
+  <dimension ref="A1:C1345"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -20360,6 +20360,2947 @@
         </is>
       </c>
     </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1dboojd</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Joining in on the trend</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dboojd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1dbondn</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Took me too long!!</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbondn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1dbo7lo</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>Any feedbacks?</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2s0yq2hc1i5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1dbnzr3</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape do you recommend for my hands? </t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbnzr3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1dbnrqd</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>new press ons🤠💅</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbnrqd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1dbn5z8</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>thoughts on chrome powder</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dbn5z8/thoughts_on_chrome_powder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1dbn140</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>first poooost (๑&gt;◡&lt;๑)</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wrn1sl6nh5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1dblpg1</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My sister finally let me do her nails! Swipe for the before. </t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dblpg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1dbmlkj</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>EDC 2024</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ir8bsvaih5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1dbmlb6</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Easy Blooming Gel Art✨</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7kenn5p7ih5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1dbml1q</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Some nails I did!</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbml1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1dbm7j5</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beautiful </t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/edix36ordh5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1dbm13v</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>My French tips!! ^O^</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tvczxwsqbh5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1dbllbp</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>monster high inspired nails wooh!</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbllbp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1dbl3sr</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>Fairy dust chrome💕</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbl3sr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1dbkrg7</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Rubber Base Help</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgy4kkpxxg5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1dbko04</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Happy Pride☺️😋</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3w8sa9xwg5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1dbkn08</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Happened a few days after my right hand, decided to shave them all down 😔</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p75w5szmwg5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1dbkme0</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made a set of press ons for my daughter </t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z5q2m6agwg5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1dbkd39</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What do y’all think </t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbkd39</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1dbk7qm</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Natural nails, regular polish</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbk7qm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1dbk5pb</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Loving my new mani</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbk5pb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1dbk1la</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Butterfly design 🦋 with encapsulated glitter ✨️ </t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbk1la</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1dbju3d</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Proud Mom</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbju3d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1dbjhvt</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>I need your advice &lt;3</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dbjhvt/i_need_your_advice_3/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1dbjf8o</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>summer nail</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cjck2ankg5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1dbjbcj</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Love this color</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbjbcj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1davpkq</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Hybrid nail polish - help needed</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1davpkq/hybrid_nail_polish_help_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1db1ima</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Can anyone help please?</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8b6zeyns9c5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1dbf9u2</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Trying again</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbf9u2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1dbfupy</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Too short for my liking but ig they are cute</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jizmg6g7nf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1dbhwsp</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Looking for sheer blue gel polish recs</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6utentov5g5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1dbhz2q</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Nirvana inspired grunge :)</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jih246h6g5d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1dbglbr</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>my take on anime nails</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbglbr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1dbis34</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Feels like summer 🍒🍉</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jqu4l90eeg5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1dbiowu</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Best matte clear polish for weak nails?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dbiowu/best_matte_clear_polish_for_weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1dbil3h</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Nail tool?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dbil3h/nail_tool/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1dbikil</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epujjprccg5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1dbihad</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Nail growth help</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbihad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1dbhj3m</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Prom press ons</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbhj3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1dbhh6w</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>I think girls will understand how hard it is to choose a color for their new manicure. But I was able to</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1445okqq1g5d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1dbhdqz</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Vacation nails ready. Hoping to be more metallic but still loving the color 😊</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vvwpz8bx0g5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1dbh7ip</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>So soft design 😍</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.redgifs.com/watch/talldefenselessurson</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1dbh5p6</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2sbc5fatyf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1dbh4qs</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🐝 beeautiful </t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eb4ccpakyf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1dbh0t9</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>Noooo</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbh0t9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1dbgxk1</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Y’all were right, independent nail techs are where it’s at 🤍</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbgxk1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1dbgww8</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>In love!</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkoiaj1iwf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1dbgwkf</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>First time using this color💜</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b0bmo4yewf5d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1dbgqqm</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>first time doing my own gel x! very proud of myself 🍒</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n9gizblzuf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1dbgop8</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>pride nails 🌈</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ui5cv0huf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1dbgerm</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm loving my current set </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m3d33b73sf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1dbgeg2</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>What’s the best nail shape on my hands?</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3k42ze0sf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1dbfxrt</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>First fancy nails as a new mom!</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbfxrt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1dbfupr</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>DIY 10</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbfupr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1dbfhqt</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Simply natural! Like it? :)</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g3d9h9yyjf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1dbe9op</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>First time doing gel x</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbe9op</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1dbe1w7</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Tried 3d nail art for the first time</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbe1w7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1dbdyj0</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Non-binary</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbdyj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1dbdsin</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>Pride nails done 🏳️‍⚧️🏳️‍🌈🏳️‍⚧️.</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbdsin</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1dbdkro</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Cute for summer 🤍</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbdkro</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1dbdesn</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>Ready for the Weekend</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbdesn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1dbdcs2</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Pearly mermaid</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0mxhrff12f5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1dbd8sg</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Checkerboard but make it fashion 🏁🏁</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbd8sg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1dbd801</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>My toxic nail trait is…</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dbd801/my_toxic_nail_trait_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1dbd5se</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Cherry Blossom Nails 💅</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbd5se</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1dbd2qe</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Had the same nail tech for years and she continues to outdo herself! </t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62y20kpnze5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1dbczbx</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>tried almond this time 😇</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pxeo629vye5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1dbcbx9</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>First time making tutorials video. What you guys think?</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u4fi2p3dte5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1dbca0a</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Milky june</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbca0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1db5odc</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Something funky</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db5odc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1db6awd</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Did I get ripped off?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xn8xu5u3gd5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1db6v3i</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tips for short/odd shaped nails? </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db6v3i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1dbc70v</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>I just did my nails opinions?</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbc70v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1db8xm8</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone ever tried Lovful? </t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1db8xm8/has_anyone_ever_tried_lovful/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1dbc5rz</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Set I did on someone else </t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/150sxg2yre5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1dba44a</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>✨The orange nails of my dreams✨🧡</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dba44a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1dbc1r1</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Any other simple mani again..</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbc1r1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1dbbqkt</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mt last two sets </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbbqkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1dbboio</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>First time using color (male)</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbboio</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1dbbjxa</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Nail day!</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbbjxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1dbbjlo</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>What’s the best nail shape for long slim fingers ?</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dbbjlo/whats_the_best_nail_shape_for_long_slim_fingers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1dbbgwp</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Asian salon</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dbbgwp/asian_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1dbbc35</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>When I want something classic but different 🤍</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ehozhi25le5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1dbb8zr</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>bi flag french for pride month!</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s9tkkyseke5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1dbb76i</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Happy pride 🌈 </t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q6on7i0zje5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1dbb3v4</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Did these a bit ago and they look better than I had anticipated? Does this look like a warm, neutral, or cool red?</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbb3v4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1dbazt7</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Happy Pride 🩷💜💙🏳️‍🌈🏳️‍⚧️</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pncmnccie5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1dbaoih</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Im just obsessed with these 💖 </t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zt909q9sfe5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1dba6oh</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What to ask for when I schedule my next appointment? </t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1dba6oh/what_to_ask_for_when_i_schedule_my_next/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1dba1lb</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Got my acrylics professionally removed today! Once I got home I applied Sally Hansen Nailgrowth Miracle…let’s see if I can kick this nail biting habit in the butt!</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1m4ecarae5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1db9113</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Sparkly floral set</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db9113</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1db8wp8</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Love love love my rainbow nails!</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lmc3o3ig1e5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1db8pfv</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Which shape looks best on me?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db8pfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1db8lnf</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>I’m in love with my work 🥹</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/phivnml2zd5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1db8j0y</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>birthday nails!🎂</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db8j0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1db891i</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>let my nail tech put any design she wanted onto my nails. how did she do??</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db891i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1db8908</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finished my pride nails! </t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db8908</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1db83d2</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>tried to make my mom happy 🥲</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db83d2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1db813a</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>considering getting gel again— would y’all recommend that after having just gotten gel removed?</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db813a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1dbnpf1</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Dazzle Dry combo</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a8nys3f9vh5d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1dbmld5</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Supportive but subtle</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbmld5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1dbl87z</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know of a good dupe for Mooncat- Malicious? </t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pozqotdv2h5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1dbkzdv</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pretty neutrals for work! </t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fc6332f70h5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1dbkbrv</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>LynB has my number and I hope she never stops calling 👉👈 (Athymy, GITD)</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbkbrv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1dbk1af</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>What do you do with a nail polish color that goes on terribly?</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dbk1af/what_do_you_do_with_a_nail_polish_color_that_goes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1dbjh8x</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Dashing Diva Carpe Diem Dupe</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbjh8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1dbj63g</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Starrily Magma has a chokehold on me</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbj63g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1dbis41</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Loving this container for my polish collection</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbis41</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1dbip6g</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Do you paint your uneven nails when growing out damage?</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dbip6g/do_you_paint_your_uneven_nails_when_growing_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1dbiihk</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>3rd ever try at painted nail art 💜🤍💚</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbiihk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1dbif4x</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Happy Pride y'all</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbif4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1dbib1s</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>this is me trying (to get a decent photo of spaceoddity)</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbib1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1dbhy2h</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>I love this color!</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbhy2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1dbhwfp</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>I don't post Pahlish often.</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbhwfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1dbhm25</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dbhm25/lurid_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1db4kxf</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Couldn't snag Trap of Love</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hcvscshc1d5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1day4s7</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>Help! Got my nails done for the first time this year, now they are damaged</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1day4s7/help_got_my_nails_done_for_the_first_time_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1dbfvn6</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>News Flash!</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dc8cptsdnf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1dbfhvw</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Btartbox Ombre Nails</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbfhvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1dbewvg</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Are you ready kids?????</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbewvg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1dbec3p</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is this look attainable with non gel polish? I can only find gel options for this pearl look </t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wajnptjcaf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1dbe97j</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Polish shaker recommendation</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dbe97j/polish_shaker_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1dbdqs4</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>My Favorite Polish</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxcf4jdg5f5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1dbdm7t</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Powder and foil recs</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dbdm7t/powder_and_foil_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1dbdjz1</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Checkerboard but make it fashion 🏁🏁</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbdjz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1dbc62w</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Mooncat A Midsummer’s Dream</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbc62w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1dbbwjq</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>Best brand at Ulta?</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dbbwjq/best_brand_at_ulta/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1dbbw1b</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Bi Nails! 💓💜💙</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbbw1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1dbbuzz</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>Magnetic tools</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dbbuzz/magnetic_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1dbbp61</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🌈 🌈 🌈 </t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbbp61</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1dbbenx</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>Y’all weren’t kidding with this one…</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wireboqle5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1dbat0n</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>MC - Ghosts of Hecate</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sk3mgtpsge5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1dbar1q</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Kitties &amp; Polish Bottles… Sigh</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1dbar1q/kitties_polish_bottles_sigh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1dba58q</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Lemon 🍋 on a Pear 🍐</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dba58q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1db8iy2</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>I’ve found my new favorite blue 🩵</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db8iy2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1db6ds6</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Birthday weekend brights</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rrexeuorgd5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1db5ppd</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new favorite vampy shade </t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db5ppd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1db5imm</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Heart of a Dying Star</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db5imm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1db58y7</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>The sage green polish of my dreams 💚</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b912n3fe7d5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1db4keb</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Can my hobbies co-exist?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e7z021nq1d5d1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1db49bh</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>🧡🏳️‍🌈Lesbian Pride🏳️‍🌈🩷</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db49bh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1db46s0</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Neons for summer? Groundbreaking </t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db46s0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1db40am</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Glowy!</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91e8gwj0xc5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1db3sql</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Matching mani to work 🌱🥬</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db3sql</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1db19f1</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Went searching for wild blueberries 🫐</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8i2bcuab7c5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1db159w</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Put your hand up if you love to do manis with mismatched hands! (polish details in comment)</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db159w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1dbo8f5</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any feedbacks? </t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29552ozm1i5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1dbmigj</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>Easy blooming gel art🤗</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u89aleqahh5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1dblsdw</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspo 💅 </t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ssmh3549h5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1dbl49t</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Heaven and Hell nails - what do you all think?</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4kwqtxym1h5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1dbksop</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>First attempt at the 3D flower💕☺️🌸</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/na4u6aabyg5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1dbklg4</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First ever character set! Bluey nails! </t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4v4v45y5wg5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1dbi2k0</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>gel ladybug nails 🐞❤️</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbi2k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1dbhtx5</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Press ons</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbhtx5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1dbhmp7</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>How do you make your stickers less stickery?</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbhmp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1dbg7jl</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Handmade manicure from Ovellaglam</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u3f8vuuaqf5d1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1dbf631</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t>Practicing look my job.</t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s3rq0npzgf5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1dbeaf6</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>I really love my pride nails 💅🏻 🫧🌈✨️💦</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/op8yepty9f5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1dbdzv6</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t>Did 3d nail art for the first time! How'd I do?</t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbdzv6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1dbdzgy</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>Non-binary</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbdzgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1dbdehf</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Checker board but make it fashion 🏁🏁</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1dbdehf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1dbc1bl</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Gold French Pearl Set. IG@NailsbyTim6</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqegvzbxqe5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1dbb0xj</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>ilove black</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ywo4dgjie5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1dbacpd</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Italian Lemon Summer Nails</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxlz6rn4de5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1db8z93</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Sparkly floral set</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db8z93</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1db8ieb</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Nail color</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0tk7fg3cyd5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1db8a9m</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Absolutely in love! </t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db8a9m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1db5zh0</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Top 10 most painful things I’ve done:</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/euc5hojjdd5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1db3be6</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Practicing nail art</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6yw2z1xqc5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1db2lzg</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>My version of tequila and citrus nails🍊</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1db2lzg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1db1hmr</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Press on nails help please!</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1db1hmr/press_on_nails_help_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1dazinp</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>I tried the 3d Pink Strawberry nails🍓 this was so fun to do!!</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u62xsn2nb5d1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>